<commit_message>
新增器件 1.AW2005 4P/5P/8P直插弯排针 2.ZXS-1191BJ弹簧顶针
</commit_message>
<xml_diff>
--- a/AD_Library/Excel/09_Connector.xlsx
+++ b/AD_Library/Excel/09_Connector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Library\AD_Library\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42313D99-91C9-4D23-9AF3-26209FD0E82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1CE091-D4FE-491B-8747-98EDA481B13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1430,7 +1430,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>POGOPING弹簧顶针-间距2.54mm-2Pin-卧贴-深圳市元升电子-POGOPING_2.54_2P_WT</t>
+    <t>POGOPING弹簧顶针-ZXS-1191BJ-间距2.54mm-2Pin-卧贴-深圳市元升电子-POGOPING_2.54_2P_WT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1808,8 +1808,8 @@
   <dimension ref="A1:U83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>